<commit_message>
added direction history data
</commit_message>
<xml_diff>
--- a/容错率.xlsx
+++ b/容错率.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M996"/>
+  <dimension ref="A1:M997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41290,6 +41290,47 @@
         <v>0.985929648241206</v>
       </c>
     </row>
+    <row r="997">
+      <c r="A997" s="1" t="n">
+        <v>995</v>
+      </c>
+      <c r="B997" t="n">
+        <v>20240313</v>
+      </c>
+      <c r="C997" t="n">
+        <v>23</v>
+      </c>
+      <c r="D997" t="n">
+        <v>39</v>
+      </c>
+      <c r="E997" t="n">
+        <v>147</v>
+      </c>
+      <c r="F997" t="n">
+        <v>226</v>
+      </c>
+      <c r="G997" t="n">
+        <v>563</v>
+      </c>
+      <c r="H997" t="n">
+        <v>991</v>
+      </c>
+      <c r="I997" t="n">
+        <v>1344</v>
+      </c>
+      <c r="J997" t="n">
+        <v>1989</v>
+      </c>
+      <c r="K997" t="n">
+        <v>101.2644578313253</v>
+      </c>
+      <c r="L997" t="n">
+        <v>6.992971887550199</v>
+      </c>
+      <c r="M997" t="n">
+        <v>0.998995983935743</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
renew history of direction
</commit_message>
<xml_diff>
--- a/容错率.xlsx
+++ b/容错率.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M1026"/>
+  <dimension ref="A1:M1027"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -42520,6 +42520,47 @@
         <v>0.2858536585365854</v>
       </c>
     </row>
+    <row r="1027">
+      <c r="A1027" s="1" t="n">
+        <v>1025</v>
+      </c>
+      <c r="B1027" t="n">
+        <v>20240426</v>
+      </c>
+      <c r="C1027" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1027" t="n">
+        <v>4</v>
+      </c>
+      <c r="E1027" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1027" t="n">
+        <v>3</v>
+      </c>
+      <c r="G1027" t="n">
+        <v>9</v>
+      </c>
+      <c r="H1027" t="n">
+        <v>20</v>
+      </c>
+      <c r="I1027" t="n">
+        <v>91</v>
+      </c>
+      <c r="J1027" t="n">
+        <v>42</v>
+      </c>
+      <c r="K1027" t="n">
+        <v>236.0212475633528</v>
+      </c>
+      <c r="L1027" t="n">
+        <v>1.510233918128655</v>
+      </c>
+      <c r="M1027" t="n">
+        <v>0.290448343079922</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>